<commit_message>
search needed multipliers from gain_setting file
</commit_message>
<xml_diff>
--- a/gain_setting.xlsx
+++ b/gain_setting.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9846FB34-ECEC-4877-B85F-8A70B32C5097}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CA8442-EFCF-8244-AEAA-FEB46AC277FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Inert</t>
   </si>
@@ -59,6 +59,36 @@
   </si>
   <si>
     <t>Factor</t>
+  </si>
+  <si>
+    <t>AMU2a</t>
+  </si>
+  <si>
+    <t>AMU17a</t>
+  </si>
+  <si>
+    <t>AMU16a</t>
+  </si>
+  <si>
+    <t>AMU4a</t>
+  </si>
+  <si>
+    <t>AMU18a</t>
+  </si>
+  <si>
+    <t>AMU29a</t>
+  </si>
+  <si>
+    <t>AMU45a</t>
+  </si>
+  <si>
+    <t>AMU30a</t>
+  </si>
+  <si>
+    <t>AMU28a</t>
+  </si>
+  <si>
+    <t>AMU32a</t>
   </si>
 </sst>
 </file>
@@ -376,19 +406,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -402,7 +432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -416,7 +446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -427,10 +457,10 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -444,7 +474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -458,7 +488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -472,7 +502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -486,7 +516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -500,7 +530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -511,10 +541,10 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -525,6 +555,146 @@
         <v>8</v>
       </c>
       <c r="D10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove `a` from `AMU32a` for multiplier search in gain setting file
</commit_message>
<xml_diff>
--- a/gain_setting.xlsx
+++ b/gain_setting.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CA8442-EFCF-8244-AEAA-FEB46AC277FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F41AD2B-CE00-294A-947D-77A7C0F9A2D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,34 +61,34 @@
     <t>Factor</t>
   </si>
   <si>
-    <t>AMU2a</t>
-  </si>
-  <si>
-    <t>AMU17a</t>
-  </si>
-  <si>
-    <t>AMU16a</t>
-  </si>
-  <si>
-    <t>AMU4a</t>
-  </si>
-  <si>
-    <t>AMU18a</t>
-  </si>
-  <si>
-    <t>AMU29a</t>
-  </si>
-  <si>
-    <t>AMU45a</t>
-  </si>
-  <si>
-    <t>AMU30a</t>
-  </si>
-  <si>
-    <t>AMU28a</t>
-  </si>
-  <si>
-    <t>AMU32a</t>
+    <t>AMU17</t>
+  </si>
+  <si>
+    <t>AMU16</t>
+  </si>
+  <si>
+    <t>AMU4</t>
+  </si>
+  <si>
+    <t>AMU18</t>
+  </si>
+  <si>
+    <t>AMU29</t>
+  </si>
+  <si>
+    <t>AMU45</t>
+  </si>
+  <si>
+    <t>AMU30</t>
+  </si>
+  <si>
+    <t>AMU28</t>
+  </si>
+  <si>
+    <t>AMU32</t>
+  </si>
+  <si>
+    <t>AMU2</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -560,7 +560,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>7</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>7</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>7</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>7</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>7</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>7</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>7</v>
@@ -658,7 +658,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>7</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>7</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>7</v>

</xml_diff>

<commit_message>
add AMU search of inert in gain setting
</commit_message>
<xml_diff>
--- a/gain_setting.xlsx
+++ b/gain_setting.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F41AD2B-CE00-294A-947D-77A7C0F9A2D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A17C27-7953-794D-B046-DB1CCEB1D406}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Inert</t>
-  </si>
-  <si>
-    <t>Reactant</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>18AMU</t>
   </si>
@@ -89,6 +83,9 @@
   </si>
   <si>
     <t>AMU2</t>
+  </si>
+  <si>
+    <t>inert</t>
   </si>
 </sst>
 </file>
@@ -406,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -420,16 +417,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -457,7 +454,7 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -513,7 +510,7 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -532,7 +529,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -541,12 +538,12 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>0.1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -560,7 +557,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>7</v>
@@ -672,30 +669,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
         <v>20</v>
-      </c>
-      <c r="B19">
-        <v>7</v>
-      </c>
-      <c r="C19">
-        <v>8</v>
-      </c>
-      <c r="D19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20">
-        <v>7</v>
-      </c>
-      <c r="C20">
-        <v>8</v>
-      </c>
-      <c r="D20">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>